<commit_message>
3.2 Atividade 4 finalizada, mas correções podem ser necessárias
</commit_message>
<xml_diff>
--- a/output/atividade4.xlsx
+++ b/output/atividade4.xlsx
@@ -618,7 +618,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.346142301140883</v>
+        <v>8.346142301140258</v>
       </c>
     </row>
     <row r="4">
@@ -673,7 +673,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q4" t="n">
-        <v>8.389234239617879</v>
+        <v>8.389234239617227</v>
       </c>
     </row>
     <row r="5">
@@ -728,7 +728,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.472275013448787</v>
+        <v>8.472275013448128</v>
       </c>
     </row>
     <row r="6">
@@ -781,7 +781,7 @@
         <v>8.595422535211267</v>
       </c>
       <c r="Q6" t="n">
-        <v>8.487999150873534</v>
+        <v>8.487999150872865</v>
       </c>
     </row>
     <row r="7">
@@ -834,7 +834,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q7" t="n">
-        <v>8.481074729780691</v>
+        <v>8.481074729780012</v>
       </c>
     </row>
     <row r="8">
@@ -887,7 +887,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q8" t="n">
-        <v>8.543761082636799</v>
+        <v>8.54376108263614</v>
       </c>
     </row>
     <row r="9">
@@ -940,7 +940,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q9" t="n">
-        <v>8.642709096785605</v>
+        <v>8.642709096784975</v>
       </c>
     </row>
     <row r="10">
@@ -993,7 +993,7 @@
         <v>8.59542253521127</v>
       </c>
       <c r="Q10" t="n">
-        <v>8.685521182937602</v>
+        <v>8.685521182937006</v>
       </c>
     </row>
     <row r="11">
@@ -1046,7 +1046,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q11" t="n">
-        <v>8.834673336044771</v>
+        <v>8.834673336044229</v>
       </c>
     </row>
     <row r="12">
@@ -1099,7 +1099,7 @@
         <v>8.59542253521127</v>
       </c>
       <c r="Q12" t="n">
-        <v>9.001753780605299</v>
+        <v>9.001753780604821</v>
       </c>
     </row>
     <row r="13">
@@ -1152,7 +1152,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q13" t="n">
-        <v>8.983378162768075</v>
+        <v>8.983378162767629</v>
       </c>
     </row>
     <row r="14">
@@ -1205,7 +1205,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q14" t="n">
-        <v>8.800845594796053</v>
+        <v>8.800845594795634</v>
       </c>
     </row>
     <row r="15">
@@ -1258,7 +1258,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q15" t="n">
-        <v>8.477375461418703</v>
+        <v>8.477375461418301</v>
       </c>
     </row>
     <row r="16">
@@ -1311,7 +1311,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q16" t="n">
-        <v>8.148497770956226</v>
+        <v>8.148497770955871</v>
       </c>
     </row>
     <row r="17">
@@ -1364,7 +1364,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q17" t="n">
-        <v>7.847523228536815</v>
+        <v>7.847523228536507</v>
       </c>
     </row>
     <row r="18">
@@ -1417,7 +1417,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q18" t="n">
-        <v>7.783638422429505</v>
+        <v>7.783638422429299</v>
       </c>
     </row>
     <row r="19">
@@ -1470,7 +1470,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q19" t="n">
-        <v>8.14724538934497</v>
+        <v>8.147245389344855</v>
       </c>
     </row>
     <row r="20">
@@ -1523,7 +1523,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q20" t="n">
-        <v>8.698297365521245</v>
+        <v>8.698297365521231</v>
       </c>
     </row>
     <row r="21">
@@ -1576,7 +1576,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q21" t="n">
-        <v>8.995850990044772</v>
+        <v>8.995850990044833</v>
       </c>
     </row>
     <row r="22">
@@ -1629,7 +1629,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q22" t="n">
-        <v>9.119020391625156</v>
+        <v>9.119020391625305</v>
       </c>
     </row>
     <row r="23">
@@ -1682,7 +1682,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q23" t="n">
-        <v>9.092985890513111</v>
+        <v>9.092985890513338</v>
       </c>
     </row>
     <row r="24">
@@ -1735,7 +1735,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q24" t="n">
-        <v>8.833848355460304</v>
+        <v>8.833848355460642</v>
       </c>
     </row>
     <row r="25">
@@ -1788,7 +1788,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q25" t="n">
-        <v>8.621238368491806</v>
+        <v>8.621238368492266</v>
       </c>
     </row>
     <row r="26">
@@ -1841,7 +1841,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q26" t="n">
-        <v>8.606113869871908</v>
+        <v>8.606113869872484</v>
       </c>
     </row>
     <row r="27">
@@ -1894,7 +1894,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q27" t="n">
-        <v>8.579714510085834</v>
+        <v>8.579714510086511</v>
       </c>
     </row>
     <row r="28">
@@ -1947,7 +1947,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q28" t="n">
-        <v>8.901809724942625</v>
+        <v>8.901809724943377</v>
       </c>
     </row>
     <row r="29">
@@ -2000,7 +2000,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q29" t="n">
-        <v>9.020665542016591</v>
+        <v>9.020665542017426</v>
       </c>
     </row>
     <row r="30">
@@ -2053,7 +2053,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q30" t="n">
-        <v>9.16874912274864</v>
+        <v>9.168749122749562</v>
       </c>
     </row>
     <row r="31">
@@ -2106,7 +2106,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q31" t="n">
-        <v>9.064027265791353</v>
+        <v>9.064027265792413</v>
       </c>
     </row>
     <row r="32">
@@ -2159,7 +2159,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q32" t="n">
-        <v>9.200121369067485</v>
+        <v>9.200121369068636</v>
       </c>
     </row>
     <row r="33">
@@ -2212,7 +2212,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q33" t="n">
-        <v>8.830578246084546</v>
+        <v>8.830578246085892</v>
       </c>
     </row>
     <row r="34">
@@ -2265,7 +2265,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q34" t="n">
-        <v>8.574287847570858</v>
+        <v>8.574287847572396</v>
       </c>
     </row>
     <row r="35">
@@ -2318,7 +2318,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q35" t="n">
-        <v>8.044293980904751</v>
+        <v>8.044293980906552</v>
       </c>
     </row>
     <row r="36">
@@ -2371,7 +2371,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q36" t="n">
-        <v>8.029127189101882</v>
+        <v>8.029127189103839</v>
       </c>
     </row>
     <row r="37">
@@ -2424,7 +2424,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q37" t="n">
-        <v>7.971537063616946</v>
+        <v>7.971537063619052</v>
       </c>
     </row>
     <row r="38">
@@ -2477,7 +2477,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q38" t="n">
-        <v>8.358886479443632</v>
+        <v>8.358886479445797</v>
       </c>
     </row>
     <row r="39">
@@ -2530,7 +2530,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q39" t="n">
-        <v>9.230217680848416</v>
+        <v>9.230217680850426</v>
       </c>
     </row>
     <row r="40">
@@ -2583,7 +2583,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q40" t="n">
-        <v>10.11659016375586</v>
+        <v>10.11659016375769</v>
       </c>
     </row>
     <row r="41">
@@ -2636,7 +2636,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q41" t="n">
-        <v>10.59265309930148</v>
+        <v>10.59265309930325</v>
       </c>
     </row>
     <row r="42">
@@ -2689,7 +2689,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q42" t="n">
-        <v>10.85640888719488</v>
+        <v>10.85640888719666</v>
       </c>
     </row>
     <row r="43">
@@ -2742,7 +2742,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q43" t="n">
-        <v>11.27503566931786</v>
+        <v>11.27503566931957</v>
       </c>
     </row>
     <row r="44">
@@ -2795,7 +2795,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q44" t="n">
-        <v>11.27627826922347</v>
+        <v>11.27627826922529</v>
       </c>
     </row>
     <row r="45">
@@ -2848,7 +2848,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q45" t="n">
-        <v>11.12089290186595</v>
+        <v>11.12089290186794</v>
       </c>
     </row>
     <row r="46">
@@ -2901,7 +2901,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q46" t="n">
-        <v>11.22648832478504</v>
+        <v>11.2264883247871</v>
       </c>
     </row>
     <row r="47">
@@ -2954,7 +2954,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q47" t="n">
-        <v>11.48735765560763</v>
+        <v>11.48735765560966</v>
       </c>
     </row>
     <row r="48">
@@ -3007,7 +3007,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q48" t="n">
-        <v>11.55726230452327</v>
+        <v>11.55726230452538</v>
       </c>
     </row>
     <row r="49">
@@ -3060,7 +3060,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q49" t="n">
-        <v>11.79783213562767</v>
+        <v>11.79783213562974</v>
       </c>
     </row>
     <row r="50">
@@ -3113,7 +3113,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q50" t="n">
-        <v>12.10155724897928</v>
+        <v>12.1015572489813</v>
       </c>
     </row>
     <row r="51">
@@ -3166,7 +3166,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q51" t="n">
-        <v>12.1057617916152</v>
+        <v>12.10576179161732</v>
       </c>
     </row>
     <row r="52">
@@ -3219,7 +3219,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q52" t="n">
-        <v>12.19012529158184</v>
+        <v>12.19012529158401</v>
       </c>
     </row>
     <row r="53">
@@ -3272,7 +3272,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q53" t="n">
-        <v>12.29721581590487</v>
+        <v>12.29721581590706</v>
       </c>
     </row>
     <row r="54">
@@ -3325,7 +3325,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q54" t="n">
-        <v>12.51574993185335</v>
+        <v>12.51574993185551</v>
       </c>
     </row>
     <row r="55">
@@ -3378,7 +3378,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q55" t="n">
-        <v>12.72166372615176</v>
+        <v>12.72166372615389</v>
       </c>
     </row>
     <row r="56">
@@ -3431,7 +3431,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q56" t="n">
-        <v>13.09535556040556</v>
+        <v>13.09535556040755</v>
       </c>
     </row>
     <row r="57">
@@ -3484,7 +3484,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q57" t="n">
-        <v>13.36602375873973</v>
+        <v>13.36602375874162</v>
       </c>
     </row>
     <row r="58">
@@ -3537,7 +3537,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q58" t="n">
-        <v>13.57305949779539</v>
+        <v>13.57305949779722</v>
       </c>
     </row>
     <row r="59">
@@ -3590,7 +3590,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q59" t="n">
-        <v>13.70250545396527</v>
+        <v>13.7025054539671</v>
       </c>
     </row>
     <row r="60">
@@ -3643,7 +3643,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q60" t="n">
-        <v>13.84447292253415</v>
+        <v>13.84447292253595</v>
       </c>
     </row>
     <row r="61">
@@ -3696,7 +3696,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q61" t="n">
-        <v>13.9010515469858</v>
+        <v>13.90105154698763</v>
       </c>
     </row>
     <row r="62">
@@ -3749,7 +3749,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q62" t="n">
-        <v>13.99806906438515</v>
+        <v>13.99806906438698</v>
       </c>
     </row>
     <row r="63">
@@ -3802,7 +3802,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q63" t="n">
-        <v>14.10758726404828</v>
+        <v>14.1075872640501</v>
       </c>
     </row>
     <row r="64">
@@ -3855,7 +3855,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q64" t="n">
-        <v>14.27233476428709</v>
+        <v>14.27233476428886</v>
       </c>
     </row>
     <row r="65">
@@ -3908,7 +3908,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q65" t="n">
-        <v>14.40745973558034</v>
+        <v>14.40745973558208</v>
       </c>
     </row>
     <row r="66">
@@ -3961,7 +3961,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q66" t="n">
-        <v>14.59524934954522</v>
+        <v>14.59524934954687</v>
       </c>
     </row>
     <row r="67">
@@ -4014,7 +4014,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q67" t="n">
-        <v>14.72910570070534</v>
+        <v>14.72910570070695</v>
       </c>
     </row>
     <row r="68">
@@ -4067,7 +4067,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q68" t="n">
-        <v>14.88190503460237</v>
+        <v>14.8819050346039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.3 Updated graphics and began Morh Circle's
</commit_message>
<xml_diff>
--- a/output/atividade4.xlsx
+++ b/output/atividade4.xlsx
@@ -618,7 +618,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.346142301140258</v>
+        <v>8.346142301140883</v>
       </c>
     </row>
     <row r="4">
@@ -673,7 +673,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q4" t="n">
-        <v>8.389234239617227</v>
+        <v>8.389234239617879</v>
       </c>
     </row>
     <row r="5">
@@ -728,7 +728,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.472275013448128</v>
+        <v>8.472275013448787</v>
       </c>
     </row>
     <row r="6">
@@ -781,7 +781,7 @@
         <v>8.595422535211267</v>
       </c>
       <c r="Q6" t="n">
-        <v>8.487999150872865</v>
+        <v>8.487999150873534</v>
       </c>
     </row>
     <row r="7">
@@ -834,7 +834,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q7" t="n">
-        <v>8.481074729780012</v>
+        <v>8.481074729780691</v>
       </c>
     </row>
     <row r="8">
@@ -887,7 +887,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q8" t="n">
-        <v>8.54376108263614</v>
+        <v>8.543761082636799</v>
       </c>
     </row>
     <row r="9">
@@ -940,7 +940,7 @@
         <v>8.595422535211268</v>
       </c>
       <c r="Q9" t="n">
-        <v>8.642709096784975</v>
+        <v>8.642709096785605</v>
       </c>
     </row>
     <row r="10">
@@ -993,7 +993,7 @@
         <v>8.59542253521127</v>
       </c>
       <c r="Q10" t="n">
-        <v>8.685521182937006</v>
+        <v>8.685521182937602</v>
       </c>
     </row>
     <row r="11">
@@ -1046,7 +1046,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q11" t="n">
-        <v>8.834673336044229</v>
+        <v>8.834673336044771</v>
       </c>
     </row>
     <row r="12">
@@ -1099,7 +1099,7 @@
         <v>8.59542253521127</v>
       </c>
       <c r="Q12" t="n">
-        <v>9.001753780604821</v>
+        <v>9.001753780605299</v>
       </c>
     </row>
     <row r="13">
@@ -1152,7 +1152,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q13" t="n">
-        <v>8.983378162767629</v>
+        <v>8.983378162768075</v>
       </c>
     </row>
     <row r="14">
@@ -1205,7 +1205,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q14" t="n">
-        <v>8.800845594795634</v>
+        <v>8.800845594796053</v>
       </c>
     </row>
     <row r="15">
@@ -1258,7 +1258,7 @@
         <v>8.595422535211272</v>
       </c>
       <c r="Q15" t="n">
-        <v>8.477375461418301</v>
+        <v>8.477375461418703</v>
       </c>
     </row>
     <row r="16">
@@ -1311,7 +1311,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q16" t="n">
-        <v>8.148497770955871</v>
+        <v>8.148497770956226</v>
       </c>
     </row>
     <row r="17">
@@ -1364,7 +1364,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q17" t="n">
-        <v>7.847523228536507</v>
+        <v>7.847523228536815</v>
       </c>
     </row>
     <row r="18">
@@ -1417,7 +1417,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q18" t="n">
-        <v>7.783638422429299</v>
+        <v>7.783638422429505</v>
       </c>
     </row>
     <row r="19">
@@ -1470,7 +1470,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q19" t="n">
-        <v>8.147245389344855</v>
+        <v>8.14724538934497</v>
       </c>
     </row>
     <row r="20">
@@ -1523,7 +1523,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q20" t="n">
-        <v>8.698297365521231</v>
+        <v>8.698297365521245</v>
       </c>
     </row>
     <row r="21">
@@ -1576,7 +1576,7 @@
         <v>8.595422535211274</v>
       </c>
       <c r="Q21" t="n">
-        <v>8.995850990044833</v>
+        <v>8.995850990044772</v>
       </c>
     </row>
     <row r="22">
@@ -1629,7 +1629,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q22" t="n">
-        <v>9.119020391625305</v>
+        <v>9.119020391625156</v>
       </c>
     </row>
     <row r="23">
@@ -1682,7 +1682,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q23" t="n">
-        <v>9.092985890513338</v>
+        <v>9.092985890513111</v>
       </c>
     </row>
     <row r="24">
@@ -1735,7 +1735,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q24" t="n">
-        <v>8.833848355460642</v>
+        <v>8.833848355460304</v>
       </c>
     </row>
     <row r="25">
@@ -1788,7 +1788,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q25" t="n">
-        <v>8.621238368492266</v>
+        <v>8.621238368491806</v>
       </c>
     </row>
     <row r="26">
@@ -1841,7 +1841,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q26" t="n">
-        <v>8.606113869872484</v>
+        <v>8.606113869871908</v>
       </c>
     </row>
     <row r="27">
@@ -1894,7 +1894,7 @@
         <v>8.595422535211275</v>
       </c>
       <c r="Q27" t="n">
-        <v>8.579714510086511</v>
+        <v>8.579714510085834</v>
       </c>
     </row>
     <row r="28">
@@ -1947,7 +1947,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q28" t="n">
-        <v>8.901809724943377</v>
+        <v>8.901809724942625</v>
       </c>
     </row>
     <row r="29">
@@ -2000,7 +2000,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q29" t="n">
-        <v>9.020665542017426</v>
+        <v>9.020665542016591</v>
       </c>
     </row>
     <row r="30">
@@ -2053,7 +2053,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q30" t="n">
-        <v>9.168749122749562</v>
+        <v>9.16874912274864</v>
       </c>
     </row>
     <row r="31">
@@ -2106,7 +2106,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q31" t="n">
-        <v>9.064027265792413</v>
+        <v>9.064027265791353</v>
       </c>
     </row>
     <row r="32">
@@ -2159,7 +2159,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q32" t="n">
-        <v>9.200121369068636</v>
+        <v>9.200121369067485</v>
       </c>
     </row>
     <row r="33">
@@ -2212,7 +2212,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q33" t="n">
-        <v>8.830578246085892</v>
+        <v>8.830578246084546</v>
       </c>
     </row>
     <row r="34">
@@ -2265,7 +2265,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q34" t="n">
-        <v>8.574287847572396</v>
+        <v>8.574287847570858</v>
       </c>
     </row>
     <row r="35">
@@ -2318,7 +2318,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q35" t="n">
-        <v>8.044293980906552</v>
+        <v>8.044293980904751</v>
       </c>
     </row>
     <row r="36">
@@ -2371,7 +2371,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q36" t="n">
-        <v>8.029127189103839</v>
+        <v>8.029127189101882</v>
       </c>
     </row>
     <row r="37">
@@ -2424,7 +2424,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q37" t="n">
-        <v>7.971537063619052</v>
+        <v>7.971537063616946</v>
       </c>
     </row>
     <row r="38">
@@ -2477,7 +2477,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q38" t="n">
-        <v>8.358886479445797</v>
+        <v>8.358886479443632</v>
       </c>
     </row>
     <row r="39">
@@ -2530,7 +2530,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q39" t="n">
-        <v>9.230217680850426</v>
+        <v>9.230217680848416</v>
       </c>
     </row>
     <row r="40">
@@ -2583,7 +2583,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q40" t="n">
-        <v>10.11659016375769</v>
+        <v>10.11659016375586</v>
       </c>
     </row>
     <row r="41">
@@ -2636,7 +2636,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q41" t="n">
-        <v>10.59265309930325</v>
+        <v>10.59265309930148</v>
       </c>
     </row>
     <row r="42">
@@ -2689,7 +2689,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q42" t="n">
-        <v>10.85640888719666</v>
+        <v>10.85640888719488</v>
       </c>
     </row>
     <row r="43">
@@ -2742,7 +2742,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q43" t="n">
-        <v>11.27503566931957</v>
+        <v>11.27503566931786</v>
       </c>
     </row>
     <row r="44">
@@ -2795,7 +2795,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q44" t="n">
-        <v>11.27627826922529</v>
+        <v>11.27627826922347</v>
       </c>
     </row>
     <row r="45">
@@ -2848,7 +2848,7 @@
         <v>8.595422535211277</v>
       </c>
       <c r="Q45" t="n">
-        <v>11.12089290186794</v>
+        <v>11.12089290186595</v>
       </c>
     </row>
     <row r="46">
@@ -2901,7 +2901,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q46" t="n">
-        <v>11.2264883247871</v>
+        <v>11.22648832478504</v>
       </c>
     </row>
     <row r="47">
@@ -2954,7 +2954,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q47" t="n">
-        <v>11.48735765560966</v>
+        <v>11.48735765560763</v>
       </c>
     </row>
     <row r="48">
@@ -3007,7 +3007,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q48" t="n">
-        <v>11.55726230452538</v>
+        <v>11.55726230452327</v>
       </c>
     </row>
     <row r="49">
@@ -3060,7 +3060,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q49" t="n">
-        <v>11.79783213562974</v>
+        <v>11.79783213562767</v>
       </c>
     </row>
     <row r="50">
@@ -3113,7 +3113,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q50" t="n">
-        <v>12.1015572489813</v>
+        <v>12.10155724897928</v>
       </c>
     </row>
     <row r="51">
@@ -3166,7 +3166,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q51" t="n">
-        <v>12.10576179161732</v>
+        <v>12.1057617916152</v>
       </c>
     </row>
     <row r="52">
@@ -3219,7 +3219,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q52" t="n">
-        <v>12.19012529158401</v>
+        <v>12.19012529158184</v>
       </c>
     </row>
     <row r="53">
@@ -3272,7 +3272,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q53" t="n">
-        <v>12.29721581590706</v>
+        <v>12.29721581590487</v>
       </c>
     </row>
     <row r="54">
@@ -3325,7 +3325,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q54" t="n">
-        <v>12.51574993185551</v>
+        <v>12.51574993185335</v>
       </c>
     </row>
     <row r="55">
@@ -3378,7 +3378,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q55" t="n">
-        <v>12.72166372615389</v>
+        <v>12.72166372615176</v>
       </c>
     </row>
     <row r="56">
@@ -3431,7 +3431,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q56" t="n">
-        <v>13.09535556040755</v>
+        <v>13.09535556040556</v>
       </c>
     </row>
     <row r="57">
@@ -3484,7 +3484,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q57" t="n">
-        <v>13.36602375874162</v>
+        <v>13.36602375873973</v>
       </c>
     </row>
     <row r="58">
@@ -3537,7 +3537,7 @@
         <v>8.595422535211279</v>
       </c>
       <c r="Q58" t="n">
-        <v>13.57305949779722</v>
+        <v>13.57305949779539</v>
       </c>
     </row>
     <row r="59">
@@ -3590,7 +3590,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q59" t="n">
-        <v>13.7025054539671</v>
+        <v>13.70250545396527</v>
       </c>
     </row>
     <row r="60">
@@ -3643,7 +3643,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q60" t="n">
-        <v>13.84447292253595</v>
+        <v>13.84447292253415</v>
       </c>
     </row>
     <row r="61">
@@ -3696,7 +3696,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q61" t="n">
-        <v>13.90105154698763</v>
+        <v>13.9010515469858</v>
       </c>
     </row>
     <row r="62">
@@ -3749,7 +3749,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q62" t="n">
-        <v>13.99806906438698</v>
+        <v>13.99806906438515</v>
       </c>
     </row>
     <row r="63">
@@ -3802,7 +3802,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q63" t="n">
-        <v>14.1075872640501</v>
+        <v>14.10758726404828</v>
       </c>
     </row>
     <row r="64">
@@ -3855,7 +3855,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q64" t="n">
-        <v>14.27233476428886</v>
+        <v>14.27233476428709</v>
       </c>
     </row>
     <row r="65">
@@ -3908,7 +3908,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q65" t="n">
-        <v>14.40745973558208</v>
+        <v>14.40745973558034</v>
       </c>
     </row>
     <row r="66">
@@ -3961,7 +3961,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q66" t="n">
-        <v>14.59524934954687</v>
+        <v>14.59524934954522</v>
       </c>
     </row>
     <row r="67">
@@ -4014,7 +4014,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q67" t="n">
-        <v>14.72910570070695</v>
+        <v>14.72910570070534</v>
       </c>
     </row>
     <row r="68">
@@ -4067,7 +4067,7 @@
         <v>8.595422535211281</v>
       </c>
       <c r="Q68" t="n">
-        <v>14.8819050346039</v>
+        <v>14.88190503460237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>